<commit_message>
Updated face detection on host application
 * Other programs which uses EgsDeviceControlCore can set "EgsDeviceSettings.IsToDetectFaces" safely.  (not tested yet)
 * Implemented ValueWithDescriptionBase, ValueWithDescription<T> and EnumValueWithDescription<T> for better auto generation of properties from excel files.
 * Updated HostApplications_Resources_Strings.xlsx and UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx.
  - Updated and re-factored EgsSourceCodeGeneration.
 * Renamed and moved functions from IsToDetectFaces to IsToDetectFacesOnDevice in EgsDeviceSettings.
 * Added FaceDetectionMethod to EgsDeviceSettings and UpdateFaceDetectionRelatedProperties() to EgsDevice.
 * Updated SettingsUserControl.xaml for face detection by host application.
 * Changed the type of some properties in EgsDeviceFaceDetectionOnHost, from double to RangedDouble.
</commit_message>
<xml_diff>
--- a/Documents/HostApplications_Resources_Strings.xlsx
+++ b/Documents/HostApplications_Resources_Strings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="826">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1"/>
@@ -4468,31 +4468,6 @@
     <t>../Windows/Projects/Egs/ZkooTutorial/Properties</t>
   </si>
   <si>
-    <t>Type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>顔検出を行うデバイス</t>
-    <rPh sb="0" eb="3">
-      <t>カオケンシュツ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>选择处理面部检测的设备</t>
-  </si>
-  <si>
-    <t>Device to Detect Faces</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>by Host Application (Higher Accuracy)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <r>
       <t>由</t>
     </r>
@@ -4507,33 +4482,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>过程在设备</t>
-  </si>
-  <si>
-    <t>デバイス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ホストアプリケーション (高精度)</t>
-    <rPh sb="13" eb="16">
-      <t>コウセイド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FaceDetectionIsProcessedByDetail</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>EgsDeviceFaceDetectionOnHost</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>(Longer Distance Needs More CPU Usage)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>by Device</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4557,10 +4510,6 @@
   </si>
   <si>
     <t>LongerDistanceNeedsMoreCpuUsage</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>进程在主机上 (更高的精度)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4592,10 +4541,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>DetectionSensitivity</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>誤検出を減らす</t>
     <rPh sb="0" eb="3">
       <t>ゴケンシュツ</t>
@@ -4666,6 +4611,38 @@
   </si>
   <si>
     <t>高特异性</t>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Max Playable Distance [m]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最大検出可能距離[m]</t>
+    <rPh sb="0" eb="2">
+      <t>サイダイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ケンシュツ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キョリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MaxPlayableDistanceInMeter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DetectionThreshold</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -4769,7 +4746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4808,16 +4785,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5138,12 +5106,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O178"/>
+  <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
+      <selection pane="bottomLeft" activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7753,7 +7721,7 @@
         <v>709</v>
       </c>
       <c r="J81" s="1" t="str">
-        <f>$F81&amp;IF(ISBLANK($G81),"","_"&amp;$G81)&amp;IF(ISBLANK($H81),"",$H81)&amp;IF(ISBLANK($I81),"","_"&amp;$I81)</f>
+        <f t="shared" ref="J81:J86" si="5">$F81&amp;IF(ISBLANK($G81),"","_"&amp;$G81)&amp;IF(ISBLANK($H81),"",$H81)&amp;IF(ISBLANK($I81),"","_"&amp;$I81)</f>
         <v>CommonStrings_Downloading</v>
       </c>
       <c r="K81" s="2"/>
@@ -7787,7 +7755,7 @@
         <v>297</v>
       </c>
       <c r="J82" s="1" t="str">
-        <f>$F82&amp;IF(ISBLANK($G82),"","_"&amp;$G82)&amp;IF(ISBLANK($H82),"",$H82)&amp;IF(ISBLANK($I82),"","_"&amp;$I82)</f>
+        <f t="shared" si="5"/>
         <v>CommonStrings_Progress</v>
       </c>
       <c r="K82" s="2"/>
@@ -7821,7 +7789,7 @@
         <v>302</v>
       </c>
       <c r="J83" s="1" t="str">
-        <f>$F83&amp;IF(ISBLANK($G83),"","_"&amp;$G83)&amp;IF(ISBLANK($H83),"",$H83)&amp;IF(ISBLANK($I83),"","_"&amp;$I83)</f>
+        <f t="shared" si="5"/>
         <v>CommonStrings_Log</v>
       </c>
       <c r="K83" s="2"/>
@@ -7852,21 +7820,21 @@
         <v>113</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="J84" s="1" t="str">
-        <f>$F84&amp;IF(ISBLANK($G84),"","_"&amp;$G84)&amp;IF(ISBLANK($H84),"",$H84)&amp;IF(ISBLANK($I84),"","_"&amp;$I84)</f>
-        <v>CommonStrings_DetectionSensitivity</v>
+        <f t="shared" si="5"/>
+        <v>CommonStrings_DetectionThreshold</v>
       </c>
       <c r="K84" s="2"/>
-      <c r="L84" s="16" t="s">
-        <v>828</v>
-      </c>
-      <c r="M84" s="16" t="s">
-        <v>829</v>
-      </c>
-      <c r="N84" s="18" t="s">
-        <v>830</v>
+      <c r="L84" s="14" t="s">
+        <v>816</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>817</v>
+      </c>
+      <c r="N84" s="15" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.4">
@@ -7886,21 +7854,21 @@
         <v>113</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>824</v>
+        <v>812</v>
       </c>
       <c r="J85" s="1" t="str">
-        <f>$F85&amp;IF(ISBLANK($G85),"","_"&amp;$G85)&amp;IF(ISBLANK($H85),"",$H85)&amp;IF(ISBLANK($I85),"","_"&amp;$I85)</f>
+        <f t="shared" si="5"/>
         <v>CommonStrings_DecreaseFalseNegativeRate</v>
       </c>
       <c r="K85" s="2"/>
-      <c r="L85" s="16" t="s">
-        <v>826</v>
-      </c>
-      <c r="M85" s="16" t="s">
-        <v>823</v>
-      </c>
-      <c r="N85" s="18" t="s">
-        <v>831</v>
+      <c r="L85" s="14" t="s">
+        <v>814</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>811</v>
+      </c>
+      <c r="N85" s="15" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.4">
@@ -7920,21 +7888,21 @@
         <v>113</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>825</v>
+        <v>813</v>
       </c>
       <c r="J86" s="1" t="str">
-        <f>$F86&amp;IF(ISBLANK($G86),"","_"&amp;$G86)&amp;IF(ISBLANK($H86),"",$H86)&amp;IF(ISBLANK($I86),"","_"&amp;$I86)</f>
+        <f t="shared" si="5"/>
         <v>CommonStrings_DecreaseFalsePositiveRate</v>
       </c>
       <c r="K86" s="2"/>
-      <c r="L86" s="16" t="s">
-        <v>827</v>
-      </c>
-      <c r="M86" s="16" t="s">
-        <v>822</v>
-      </c>
-      <c r="N86" s="18" t="s">
-        <v>832</v>
+      <c r="L86" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>810</v>
+      </c>
+      <c r="N86" s="15" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.4">
@@ -8182,7 +8150,7 @@
         <v>226</v>
       </c>
       <c r="J93" s="1" t="str">
-        <f t="shared" ref="J93:J136" si="5">$F93&amp;IF(ISBLANK($G93),"","_"&amp;$G93)&amp;IF(ISBLANK($H93),"",$H93)&amp;IF(ISBLANK($I93),"","_"&amp;$I93)</f>
+        <f t="shared" ref="J93:J134" si="6">$F93&amp;IF(ISBLANK($G93),"","_"&amp;$G93)&amp;IF(ISBLANK($H93),"",$H93)&amp;IF(ISBLANK($I93),"","_"&amp;$I93)</f>
         <v>CameraViewWindowModel_CanDragMove_Description</v>
       </c>
       <c r="K93" s="2"/>
@@ -8222,7 +8190,7 @@
         <v>226</v>
       </c>
       <c r="J94" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CameraViewWindowModel_CanDragMoveEnabled_Description</v>
       </c>
       <c r="K94" s="2"/>
@@ -8262,7 +8230,7 @@
         <v>226</v>
       </c>
       <c r="J95" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CameraViewWindowModel_CanDragMoveDisabled_Description</v>
       </c>
       <c r="K95" s="2"/>
@@ -8299,7 +8267,7 @@
         <v>226</v>
       </c>
       <c r="J96" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CameraViewWindowModel_CanResize_Description</v>
       </c>
       <c r="K96" s="2"/>
@@ -8336,7 +8304,7 @@
         <v>226</v>
       </c>
       <c r="J97" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CameraViewWindowModel_CanShowMenu_Description</v>
       </c>
       <c r="K97" s="2"/>
@@ -8373,7 +8341,7 @@
         <v>226</v>
       </c>
       <c r="J98" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CameraViewWindowModel_Topmost_Description</v>
       </c>
       <c r="K98" s="2"/>
@@ -8410,7 +8378,7 @@
         <v>226</v>
       </c>
       <c r="J99" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>CameraViewWindowModel_WindowStateControlMethodSetByUser_Description</v>
       </c>
       <c r="K99" s="2"/>
@@ -8478,7 +8446,7 @@
         <v>376</v>
       </c>
       <c r="J101" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_DeviceFirmwareUpdate</v>
       </c>
       <c r="K101" s="2"/>
@@ -8512,7 +8480,7 @@
         <v>380</v>
       </c>
       <c r="J102" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_PleaseUpdateDeviceFirmware</v>
       </c>
       <c r="K102" s="2"/>
@@ -8546,7 +8514,7 @@
         <v>383</v>
       </c>
       <c r="J103" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_DoNotDisconnectTheDevice</v>
       </c>
       <c r="K103" s="2"/>
@@ -8580,7 +8548,7 @@
         <v>387</v>
       </c>
       <c r="J104" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_ZkooNeedsReboot</v>
       </c>
       <c r="K104" s="2"/>
@@ -8614,7 +8582,7 @@
         <v>391</v>
       </c>
       <c r="J105" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_ZkooNeedsToDisconnectPowerCable</v>
       </c>
       <c r="K105" s="2"/>
@@ -8648,7 +8616,7 @@
         <v>395</v>
       </c>
       <c r="J106" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_ZkooNeedsToConnectPowerCable</v>
       </c>
       <c r="K106" s="2"/>
@@ -8682,7 +8650,7 @@
         <v>399</v>
       </c>
       <c r="J107" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_DfuImageFileIsInvalid</v>
       </c>
       <c r="K107" s="2"/>
@@ -8716,7 +8684,7 @@
         <v>403</v>
       </c>
       <c r="J108" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_DfuCanceled</v>
       </c>
       <c r="K108" s="2"/>
@@ -8750,7 +8718,7 @@
         <v>407</v>
       </c>
       <c r="J109" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_RestartDfuFromBeginning</v>
       </c>
       <c r="K109" s="2"/>
@@ -8784,7 +8752,7 @@
         <v>410</v>
       </c>
       <c r="J110" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_DfuFailed</v>
       </c>
       <c r="K110" s="2"/>
@@ -8818,7 +8786,7 @@
         <v>414</v>
       </c>
       <c r="J111" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_AppWillRetrySendingImageAgain</v>
       </c>
       <c r="K111" s="2"/>
@@ -8852,7 +8820,7 @@
         <v>418</v>
       </c>
       <c r="J112" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>EgsDeviceFirmwareUpdateModel_DfuCompleted</v>
       </c>
       <c r="K112" s="2"/>
@@ -8889,7 +8857,7 @@
         <v>226</v>
       </c>
       <c r="J113" s="1" t="str">
-        <f t="shared" ref="J113:J119" si="6">$F113&amp;IF(ISBLANK($G113),"","_"&amp;$G113)&amp;IF(ISBLANK($H113),"",$H113)&amp;IF(ISBLANK($I113),"","_"&amp;$I113)</f>
+        <f t="shared" ref="J113:J117" si="7">$F113&amp;IF(ISBLANK($G113),"","_"&amp;$G113)&amp;IF(ISBLANK($H113),"",$H113)&amp;IF(ISBLANK($I113),"","_"&amp;$I113)</f>
         <v>CameraViewBordersAndPointersAreDrawnByDetail_Type_Description</v>
       </c>
       <c r="K113" s="2"/>
@@ -8926,7 +8894,7 @@
         <v>226</v>
       </c>
       <c r="J114" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>CameraViewBordersAndPointersAreDrawnByDetail_ByHostApplication_Description</v>
       </c>
       <c r="K114" s="2"/>
@@ -8963,7 +8931,7 @@
         <v>226</v>
       </c>
       <c r="J115" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>CameraViewBordersAndPointersAreDrawnByDetail_ByDevice_Description</v>
       </c>
       <c r="K115" s="2"/>
@@ -8974,12 +8942,12 @@
         <v>435</v>
       </c>
       <c r="N115" s="5" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>394</v>
+        <v>459</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>112</v>
@@ -8988,35 +8956,32 @@
         <v>802</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>422</v>
+        <v>15</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>226</v>
+        <v>808</v>
       </c>
       <c r="J116" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>FaceDetectionIsProcessedByDetail_Type_Description</v>
+        <f t="shared" si="7"/>
+        <v>EgsDeviceFaceDetectionOnHost_LongerDistanceNeedsMoreCpuUsage</v>
       </c>
       <c r="K116" s="2"/>
       <c r="L116" s="14" t="s">
+        <v>806</v>
+      </c>
+      <c r="M116" s="14" t="s">
         <v>807</v>
       </c>
-      <c r="M116" s="14" t="s">
-        <v>805</v>
-      </c>
-      <c r="N116" s="15" t="s">
-        <v>806</v>
+      <c r="N116" s="14" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>112</v>
@@ -9025,35 +8990,35 @@
         <v>802</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>422</v>
+        <v>15</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>428</v>
+        <v>824</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>226</v>
+        <v>821</v>
       </c>
       <c r="J117" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>FaceDetectionIsProcessedByDetail_ByHostApplication_Description</v>
+        <f t="shared" si="7"/>
+        <v>EgsDeviceFaceDetectionOnHost_MaxPlayableDistanceInMeter_Description</v>
       </c>
       <c r="K117" s="2"/>
-      <c r="L117" s="16" t="s">
-        <v>808</v>
-      </c>
-      <c r="M117" s="16" t="s">
-        <v>812</v>
-      </c>
-      <c r="N117" s="17" t="s">
-        <v>819</v>
+      <c r="L117" s="14" t="s">
+        <v>822</v>
+      </c>
+      <c r="M117" s="14" t="s">
+        <v>823</v>
+      </c>
+      <c r="N117" s="14" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>112</v>
@@ -9065,32 +9030,32 @@
         <v>422</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>813</v>
+        <v>437</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J118" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>FaceDetectionIsProcessedByDetail_ByDevice_Description</v>
+        <v>CultureInfoAndDescriptionDetail_Type_Description</v>
       </c>
       <c r="K118" s="2"/>
-      <c r="L118" s="16" t="s">
-        <v>816</v>
-      </c>
-      <c r="M118" s="16" t="s">
-        <v>811</v>
-      </c>
-      <c r="N118" s="17" t="s">
-        <v>810</v>
+      <c r="L118" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="M118" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="N118" s="5" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>112</v>
@@ -9099,32 +9064,35 @@
         <v>802</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>15</v>
+        <v>422</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>814</v>
+        <v>437</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>818</v>
+        <v>441</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="J119" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>EgsDeviceFaceDetectionOnHost_LongerDistanceNeedsMoreCpuUsage</v>
+        <v>CultureInfoAndDescriptionDetail_UseOSCulture_Description</v>
       </c>
       <c r="K119" s="2"/>
-      <c r="L119" s="16" t="s">
-        <v>815</v>
-      </c>
-      <c r="M119" s="16" t="s">
-        <v>817</v>
-      </c>
-      <c r="N119" s="16" t="s">
-        <v>820</v>
+      <c r="L119" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="M119" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="N119" s="5" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>112</v>
@@ -9136,32 +9104,32 @@
         <v>422</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J120" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CultureInfoAndDescriptionDetail_Type_Description</v>
+        <f t="shared" si="6"/>
+        <v>CultureInfoAndDescriptionDetail_English_Description</v>
       </c>
       <c r="K120" s="2"/>
       <c r="L120" s="9" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="M120" s="9" t="s">
-        <v>439</v>
-      </c>
-      <c r="N120" s="5" t="s">
-        <v>788</v>
+        <v>447</v>
+      </c>
+      <c r="N120" s="12" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>112</v>
@@ -9173,32 +9141,32 @@
         <v>422</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J121" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CultureInfoAndDescriptionDetail_UseOSCulture_Description</v>
+        <f t="shared" si="6"/>
+        <v>CultureInfoAndDescriptionDetail_Japanese_Description</v>
       </c>
       <c r="K121" s="2"/>
       <c r="L121" s="9" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="M121" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="N121" s="5" t="s">
-        <v>444</v>
+        <v>450</v>
+      </c>
+      <c r="N121" s="12" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>112</v>
@@ -9213,29 +9181,29 @@
         <v>446</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="I122" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J122" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CultureInfoAndDescriptionDetail_English_Description</v>
+        <f t="shared" si="6"/>
+        <v>CultureInfoAndDescriptionDetail_Chinese_Description</v>
       </c>
       <c r="K122" s="2"/>
-      <c r="L122" s="9" t="s">
-        <v>447</v>
-      </c>
-      <c r="M122" s="9" t="s">
-        <v>447</v>
-      </c>
-      <c r="N122" s="12" t="s">
-        <v>447</v>
+      <c r="L122" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="M122" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="N122" s="5" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>112</v>
@@ -9247,32 +9215,32 @@
         <v>422</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="I123" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J123" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CultureInfoAndDescriptionDetail_Japanese_Description</v>
+        <f t="shared" si="6"/>
+        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_Type_Description</v>
       </c>
       <c r="K123" s="2"/>
       <c r="L123" s="9" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="M123" s="9" t="s">
-        <v>450</v>
-      </c>
-      <c r="N123" s="12" t="s">
-        <v>450</v>
+        <v>458</v>
+      </c>
+      <c r="N123" s="5" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>112</v>
@@ -9284,32 +9252,32 @@
         <v>422</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J124" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CultureInfoAndDescriptionDetail_Chinese_Description</v>
+        <f t="shared" si="6"/>
+        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_None_Description</v>
       </c>
       <c r="K124" s="2"/>
-      <c r="L124" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="M124" s="11" t="s">
-        <v>453</v>
+      <c r="L124" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="M124" s="9" t="s">
+        <v>461</v>
       </c>
       <c r="N124" s="5" t="s">
-        <v>454</v>
+        <v>705</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>112</v>
@@ -9324,29 +9292,29 @@
         <v>456</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>424</v>
+        <v>463</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J125" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_Type_Description</v>
+        <f t="shared" si="6"/>
+        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_FirstFoundHand_Description</v>
       </c>
       <c r="K125" s="2"/>
       <c r="L125" s="9" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="M125" s="9" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="N125" s="5" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>112</v>
@@ -9361,29 +9329,29 @@
         <v>456</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="I126" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J126" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_None_Description</v>
+        <f t="shared" si="6"/>
+        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_RightHand_Description</v>
       </c>
       <c r="K126" s="2"/>
       <c r="L126" s="9" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="M126" s="9" t="s">
-        <v>461</v>
-      </c>
-      <c r="N126" s="5" t="s">
-        <v>705</v>
+        <v>469</v>
+      </c>
+      <c r="N126" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A127" s="2" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>112</v>
@@ -9398,29 +9366,29 @@
         <v>456</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J127" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_FirstFoundHand_Description</v>
+        <f t="shared" si="6"/>
+        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_LeftHand_Description</v>
       </c>
       <c r="K127" s="2"/>
       <c r="L127" s="9" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="M127" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="N127" s="5" t="s">
-        <v>707</v>
+        <v>474</v>
+      </c>
+      <c r="N127" s="12" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A128" s="2" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>112</v>
@@ -9432,32 +9400,32 @@
         <v>422</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>456</v>
+        <v>477</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>467</v>
+        <v>424</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J128" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_RightHand_Description</v>
+        <f t="shared" si="6"/>
+        <v>CursorDrawingTimingMethodDetail_Type_Description</v>
       </c>
       <c r="K128" s="2"/>
       <c r="L128" s="9" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="M128" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="N128" s="12" t="s">
-        <v>470</v>
+        <v>479</v>
+      </c>
+      <c r="N128" s="5" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A129" s="2" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>112</v>
@@ -9469,32 +9437,32 @@
         <v>422</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>456</v>
+        <v>477</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J129" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseCursorPositionUpdatedByGestureCursorMethodDetail_LeftHand_Description</v>
+        <f t="shared" si="6"/>
+        <v>CursorDrawingTimingMethodDetail_ByHidReportUpdatedEvent_Description</v>
       </c>
       <c r="K129" s="2"/>
       <c r="L129" s="9" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="M129" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="N129" s="12" t="s">
-        <v>475</v>
+        <v>484</v>
+      </c>
+      <c r="N129" s="5" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A130" s="2" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>112</v>
@@ -9506,32 +9474,32 @@
         <v>422</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>424</v>
+        <v>488</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J130" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CursorDrawingTimingMethodDetail_Type_Description</v>
+        <f t="shared" si="6"/>
+        <v>CursorDrawingTimingMethodDetail_ByTimer60Fps_Description</v>
       </c>
       <c r="K130" s="2"/>
       <c r="L130" s="9" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="M130" s="9" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="N130" s="5" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A131" s="2" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>112</v>
@@ -9543,32 +9511,32 @@
         <v>422</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>482</v>
+        <v>492</v>
       </c>
       <c r="I131" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J131" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CursorDrawingTimingMethodDetail_ByHidReportUpdatedEvent_Description</v>
+        <f t="shared" si="6"/>
+        <v>CursorDrawingTimingMethodDetail_ByTimer30Fps_Description</v>
       </c>
       <c r="K131" s="2"/>
       <c r="L131" s="9" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
       <c r="M131" s="9" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="N131" s="5" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A132" s="2" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>112</v>
@@ -9580,32 +9548,32 @@
         <v>422</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>488</v>
+        <v>424</v>
       </c>
       <c r="I132" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J132" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CursorDrawingTimingMethodDetail_ByTimer60Fps_Description</v>
+        <f t="shared" si="6"/>
+        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_Type_Description</v>
       </c>
       <c r="K132" s="2"/>
       <c r="L132" s="9" t="s">
-        <v>489</v>
+        <v>676</v>
       </c>
       <c r="M132" s="9" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="N132" s="5" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A133" s="2" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>112</v>
@@ -9617,32 +9585,32 @@
         <v>422</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="I133" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J133" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CursorDrawingTimingMethodDetail_ByTimer30Fps_Description</v>
+        <f t="shared" si="6"/>
+        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_UseUsersControlMethods_Description</v>
       </c>
       <c r="K133" s="2"/>
       <c r="L133" s="9" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="M133" s="9" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="N133" s="5" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A134" s="2" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>112</v>
@@ -9657,29 +9625,29 @@
         <v>495</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>424</v>
+        <v>504</v>
       </c>
       <c r="I134" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J134" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_Type_Description</v>
+        <f t="shared" si="6"/>
+        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_KeepNormal_Description</v>
       </c>
       <c r="K134" s="2"/>
       <c r="L134" s="9" t="s">
-        <v>676</v>
+        <v>505</v>
       </c>
       <c r="M134" s="9" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="N134" s="5" t="s">
-        <v>497</v>
+        <v>761</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A135" s="2" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>112</v>
@@ -9694,29 +9662,29 @@
         <v>495</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>499</v>
+        <v>508</v>
       </c>
       <c r="I135" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J135" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_UseUsersControlMethods_Description</v>
+        <f t="shared" ref="J135:J167" si="8">$F135&amp;IF(ISBLANK($G135),"","_"&amp;$G135)&amp;IF(ISBLANK($H135),"",$H135)&amp;IF(ISBLANK($I135),"","_"&amp;$I135)</f>
+        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_KeepMinimized_Description</v>
       </c>
       <c r="K135" s="2"/>
       <c r="L135" s="9" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="M135" s="9" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="N135" s="5" t="s">
-        <v>502</v>
+        <v>697</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A136" s="2" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>112</v>
@@ -9728,32 +9696,32 @@
         <v>422</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>495</v>
+        <v>512</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>504</v>
+        <v>424</v>
       </c>
       <c r="I136" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J136" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_KeepNormal_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_Type_Description</v>
       </c>
       <c r="K136" s="2"/>
       <c r="L136" s="9" t="s">
-        <v>505</v>
+        <v>677</v>
       </c>
       <c r="M136" s="9" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="N136" s="5" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.4">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A137" s="2" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>112</v>
@@ -9765,32 +9733,32 @@
         <v>422</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>495</v>
+        <v>512</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="I137" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J137" s="1" t="str">
-        <f t="shared" ref="J137:J169" si="7">$F137&amp;IF(ISBLANK($G137),"","_"&amp;$G137)&amp;IF(ISBLANK($H137),"",$H137)&amp;IF(ISBLANK($I137),"","_"&amp;$I137)</f>
-        <v>CameraViewWindowStateHostApplicationsControlMethodDetail_KeepMinimized_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ManualOnOff_Description</v>
       </c>
       <c r="K137" s="2"/>
       <c r="L137" s="9" t="s">
-        <v>509</v>
+        <v>678</v>
       </c>
       <c r="M137" s="9" t="s">
-        <v>510</v>
+        <v>679</v>
       </c>
       <c r="N137" s="5" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.4">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A138" s="2" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>112</v>
@@ -9805,29 +9773,29 @@
         <v>512</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>424</v>
+        <v>517</v>
       </c>
       <c r="I138" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J138" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_Type_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenFaceDetectionStarts_HideSoonAfterHandTrackingStarts_Description</v>
       </c>
       <c r="K138" s="2"/>
       <c r="L138" s="9" t="s">
-        <v>677</v>
+        <v>518</v>
       </c>
       <c r="M138" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="N138" s="5" t="s">
-        <v>698</v>
+        <v>519</v>
+      </c>
+      <c r="N138" s="8" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A139" s="2" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>112</v>
@@ -9842,29 +9810,29 @@
         <v>512</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="I139" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J139" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ManualOnOff_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenFaceDetectionStarts_HideSoonAfterHandDetectionStarts_ShowWhenHandTrackingStarts_Description</v>
       </c>
       <c r="K139" s="2"/>
-      <c r="L139" s="9" t="s">
-        <v>678</v>
+      <c r="L139" s="10" t="s">
+        <v>680</v>
       </c>
       <c r="M139" s="9" t="s">
-        <v>679</v>
+        <v>523</v>
       </c>
       <c r="N139" s="5" t="s">
-        <v>762</v>
+        <v>699</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A140" s="2" t="s">
-        <v>538</v>
+        <v>547</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>112</v>
@@ -9879,29 +9847,29 @@
         <v>512</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="I140" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J140" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenFaceDetectionStarts_HideSoonAfterHandTrackingStarts_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenFaceDetectionStarts_HideSoonAfterHandDetectionStarts_ShowWhenHandTrackingStarts_HideSoonAfterHandTrackingStarts_Description</v>
       </c>
       <c r="K140" s="2"/>
-      <c r="L140" s="9" t="s">
-        <v>518</v>
+      <c r="L140" s="10" t="s">
+        <v>681</v>
       </c>
       <c r="M140" s="9" t="s">
-        <v>519</v>
-      </c>
-      <c r="N140" s="8" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
+        <v>686</v>
+      </c>
+      <c r="N140" s="5" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A141" s="2" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>112</v>
@@ -9916,29 +9884,29 @@
         <v>512</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="I141" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J141" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenFaceDetectionStarts_HideSoonAfterHandDetectionStarts_ShowWhenHandTrackingStarts_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandDetectionStarts_HideWhenHandDetectionEnds_HideWhenHandTrackingEnds_Description</v>
       </c>
       <c r="K141" s="2"/>
       <c r="L141" s="10" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="M141" s="9" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="N141" s="5" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A142" s="2" t="s">
-        <v>547</v>
+        <v>556</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>112</v>
@@ -9953,29 +9921,29 @@
         <v>512</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="I142" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J142" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenFaceDetectionStarts_HideSoonAfterHandDetectionStarts_ShowWhenHandTrackingStarts_HideSoonAfterHandTrackingStarts_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandDetectionStarts_HideWhenHandDetectionEnds_HideSoonAfterHandTrackingStarts_Description</v>
       </c>
       <c r="K142" s="2"/>
       <c r="L142" s="10" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M142" s="9" t="s">
-        <v>686</v>
+        <v>531</v>
       </c>
       <c r="N142" s="5" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A143" s="2" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>112</v>
@@ -9990,29 +9958,29 @@
         <v>512</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="I143" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J143" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandDetectionStarts_HideWhenHandDetectionEnds_HideWhenHandTrackingEnds_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandTrackingStarts_HideWhenHandTrackingEnds_Description</v>
       </c>
       <c r="K143" s="2"/>
       <c r="L143" s="10" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="M143" s="9" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="N143" s="5" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A144" s="2" t="s">
-        <v>556</v>
+        <v>565</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>112</v>
@@ -10027,29 +9995,29 @@
         <v>512</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="I144" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J144" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandDetectionStarts_HideWhenHandDetectionEnds_HideSoonAfterHandTrackingStarts_Description</v>
+        <f t="shared" si="8"/>
+        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandTrackingStarts_HideSoonAfterHandTrackingStarts_Description</v>
       </c>
       <c r="K144" s="2"/>
       <c r="L144" s="10" t="s">
-        <v>683</v>
+        <v>537</v>
       </c>
       <c r="M144" s="9" t="s">
-        <v>531</v>
+        <v>685</v>
       </c>
       <c r="N144" s="5" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A145" s="2" t="s">
-        <v>560</v>
+        <v>569</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>112</v>
@@ -10058,35 +10026,35 @@
         <v>802</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>422</v>
+        <v>539</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>512</v>
+        <v>540</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="I145" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J145" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandTrackingStarts_HideWhenHandTrackingEnds_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_BasicSettings_Description</v>
       </c>
       <c r="K145" s="2"/>
-      <c r="L145" s="10" t="s">
-        <v>684</v>
+      <c r="L145" s="9" t="s">
+        <v>542</v>
       </c>
       <c r="M145" s="9" t="s">
-        <v>534</v>
+        <v>543</v>
       </c>
       <c r="N145" s="5" t="s">
-        <v>703</v>
+        <v>544</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A146" s="2" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>112</v>
@@ -10095,35 +10063,35 @@
         <v>802</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>422</v>
+        <v>539</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>512</v>
+        <v>540</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="I146" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J146" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>CameraViewWindowStateUsersControlMethodDetail_ShowWhenHandTrackingStarts_HideSoonAfterHandTrackingStarts_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_CameraViewSettings_Description</v>
       </c>
       <c r="K146" s="2"/>
-      <c r="L146" s="10" t="s">
-        <v>537</v>
+      <c r="L146" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="M146" s="9" t="s">
-        <v>685</v>
+        <v>222</v>
       </c>
       <c r="N146" s="5" t="s">
-        <v>704</v>
+        <v>223</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A147" s="2" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>112</v>
@@ -10138,29 +10106,29 @@
         <v>540</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="I147" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J147" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_BasicSettings_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_AdvancedSettings_Description</v>
       </c>
       <c r="K147" s="2"/>
       <c r="L147" s="9" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="M147" s="9" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="N147" s="5" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A148" s="2" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>112</v>
@@ -10175,29 +10143,29 @@
         <v>540</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="I148" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J148" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_CameraViewSettings_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_DeveloperSettings_Description</v>
       </c>
       <c r="K148" s="2"/>
       <c r="L148" s="9" t="s">
-        <v>221</v>
+        <v>554</v>
       </c>
       <c r="M148" s="9" t="s">
-        <v>222</v>
+        <v>555</v>
       </c>
       <c r="N148" s="5" t="s">
-        <v>223</v>
+        <v>789</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A149" s="2" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>112</v>
@@ -10212,29 +10180,29 @@
         <v>540</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>548</v>
+        <v>557</v>
       </c>
       <c r="I149" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J149" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_AdvancedSettings_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_ExvisionSettings_Description</v>
       </c>
       <c r="K149" s="2"/>
       <c r="L149" s="9" t="s">
-        <v>549</v>
+        <v>558</v>
       </c>
       <c r="M149" s="9" t="s">
-        <v>550</v>
+        <v>559</v>
       </c>
       <c r="N149" s="5" t="s">
-        <v>551</v>
+        <v>790</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A150" s="2" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>112</v>
@@ -10249,29 +10217,29 @@
         <v>540</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="I150" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J150" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_DeveloperSettings_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_TutorialAppSettings_Description</v>
       </c>
       <c r="K150" s="2"/>
       <c r="L150" s="9" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
       <c r="M150" s="9" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="N150" s="5" t="s">
-        <v>789</v>
+        <v>564</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A151" s="2" t="s">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>112</v>
@@ -10286,29 +10254,29 @@
         <v>540</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>557</v>
+        <v>566</v>
       </c>
       <c r="I151" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J151" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_ExvisionSettings_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_StartTutorial_Description</v>
       </c>
       <c r="K151" s="2"/>
       <c r="L151" s="9" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="M151" s="9" t="s">
-        <v>559</v>
+        <v>568</v>
       </c>
       <c r="N151" s="5" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A152" s="2" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>112</v>
@@ -10323,29 +10291,29 @@
         <v>540</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>561</v>
+        <v>570</v>
       </c>
       <c r="I152" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J152" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_TutorialAppSettings_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_OptionsForLowerSpecPc_Description</v>
       </c>
       <c r="K152" s="2"/>
       <c r="L152" s="9" t="s">
-        <v>562</v>
+        <v>571</v>
       </c>
       <c r="M152" s="9" t="s">
-        <v>563</v>
+        <v>763</v>
       </c>
       <c r="N152" s="5" t="s">
-        <v>564</v>
+        <v>765</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A153" s="2" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>112</v>
@@ -10360,103 +10328,97 @@
         <v>540</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="I153" s="2" t="s">
         <v>226</v>
       </c>
       <c r="J153" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_StartTutorial_Description</v>
+        <f t="shared" si="8"/>
+        <v>SettingsUserControl_AnalogGain_Description</v>
       </c>
       <c r="K153" s="2"/>
       <c r="L153" s="9" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="M153" s="9" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="N153" s="5" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A154" s="2" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>112</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>539</v>
+        <v>577</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="I154" s="2" t="s">
-        <v>226</v>
+        <v>578</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>756</v>
       </c>
       <c r="J154" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_OptionsForLowerSpecPc_Description</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_TutorialWindowTitle</v>
       </c>
       <c r="K154" s="2"/>
       <c r="L154" s="9" t="s">
-        <v>571</v>
+        <v>755</v>
       </c>
       <c r="M154" s="9" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="N154" s="5" t="s">
-        <v>765</v>
+        <v>754</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A155" s="2" t="s">
-        <v>608</v>
+        <v>617</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>112</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>539</v>
+        <v>577</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="I155" s="2" t="s">
-        <v>226</v>
+        <v>578</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>579</v>
       </c>
       <c r="J155" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>SettingsUserControl_AnalogGain_Description</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_EndUserLicenseAgreement</v>
       </c>
       <c r="K155" s="2"/>
       <c r="L155" s="9" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="M155" s="9" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="N155" s="5" t="s">
-        <v>792</v>
+        <v>582</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A156" s="2" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>112</v>
@@ -10471,26 +10433,26 @@
         <v>578</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>756</v>
+        <v>584</v>
       </c>
       <c r="J156" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_TutorialWindowTitle</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_PrivacyPolicy</v>
       </c>
       <c r="K156" s="2"/>
       <c r="L156" s="9" t="s">
-        <v>755</v>
+        <v>585</v>
       </c>
       <c r="M156" s="9" t="s">
-        <v>753</v>
+        <v>586</v>
       </c>
       <c r="N156" s="5" t="s">
-        <v>754</v>
+        <v>587</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A157" s="2" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>112</v>
@@ -10505,26 +10467,26 @@
         <v>578</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="J157" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_EndUserLicenseAgreement</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_IAcceptTheEula</v>
       </c>
       <c r="K157" s="2"/>
       <c r="L157" s="9" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="M157" s="9" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="N157" s="5" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A158" s="2" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>112</v>
@@ -10539,26 +10501,26 @@
         <v>578</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="J158" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_PrivacyPolicy</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_BySelectingNext_YouAgreeToExvisions</v>
       </c>
       <c r="K158" s="2"/>
       <c r="L158" s="9" t="s">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="M158" s="9" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="N158" s="5" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A159" s="2" t="s">
-        <v>625</v>
+        <v>632</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>112</v>
@@ -10572,27 +10534,27 @@
       <c r="F159" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G159" s="3" t="s">
-        <v>589</v>
+      <c r="G159" s="1" t="s">
+        <v>599</v>
       </c>
       <c r="J159" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_IAcceptTheEula</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_LetsStartTutorials</v>
       </c>
       <c r="K159" s="2"/>
       <c r="L159" s="9" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="M159" s="9" t="s">
-        <v>591</v>
+        <v>601</v>
       </c>
       <c r="N159" s="5" t="s">
-        <v>592</v>
+        <v>602</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A160" s="2" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>112</v>
@@ -10606,27 +10568,27 @@
       <c r="F160" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G160" s="3" t="s">
-        <v>594</v>
+      <c r="G160" s="1" t="s">
+        <v>604</v>
       </c>
       <c r="J160" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_BySelectingNext_YouAgreeToExvisions</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_FailedToPlayAVideo</v>
       </c>
       <c r="K160" s="2"/>
       <c r="L160" s="9" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
       <c r="M160" s="9" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="N160" s="5" t="s">
-        <v>597</v>
+        <v>607</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A161" s="2" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>112</v>
@@ -10641,26 +10603,26 @@
         <v>578</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="J161" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_LetsStartTutorials</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_ZkooTutorialIsStarting</v>
       </c>
       <c r="K161" s="2"/>
       <c r="L161" s="9" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="M161" s="9" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
       <c r="N161" s="5" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A162" s="2" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>112</v>
@@ -10675,26 +10637,26 @@
         <v>578</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="J162" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_FailedToPlayAVideo</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_ZkooTutorialNeedsInternetConnections</v>
       </c>
       <c r="K162" s="2"/>
       <c r="L162" s="9" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="M162" s="9" t="s">
-        <v>606</v>
+        <v>616</v>
       </c>
       <c r="N162" s="5" t="s">
-        <v>607</v>
+        <v>793</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A163" s="2" t="s">
-        <v>642</v>
+        <v>652</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>112</v>
@@ -10708,27 +10670,27 @@
       <c r="F163" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G163" s="1" t="s">
-        <v>609</v>
+      <c r="G163" s="3" t="s">
+        <v>618</v>
       </c>
       <c r="J163" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_ZkooTutorialIsStarting</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_Replay</v>
       </c>
       <c r="K163" s="2"/>
       <c r="L163" s="9" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="M163" s="9" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="N163" s="5" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A164" s="2" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>112</v>
@@ -10742,27 +10704,27 @@
       <c r="F164" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G164" s="1" t="s">
-        <v>614</v>
+      <c r="G164" s="3" t="s">
+        <v>622</v>
       </c>
       <c r="J164" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_ZkooTutorialNeedsInternetConnections</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_Video</v>
       </c>
       <c r="K164" s="2"/>
       <c r="L164" s="9" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="M164" s="9" t="s">
-        <v>616</v>
+        <v>623</v>
       </c>
       <c r="N164" s="5" t="s">
-        <v>793</v>
+        <v>624</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A165" s="2" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>112</v>
@@ -10777,18 +10739,18 @@
         <v>578</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="J165" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_Replay</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_Retry</v>
       </c>
       <c r="K165" s="2"/>
       <c r="L165" s="9" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="M165" s="9" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="N165" s="5" t="s">
         <v>620</v>
@@ -10796,7 +10758,7 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A166" s="2" t="s">
-        <v>657</v>
+        <v>666</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>112</v>
@@ -10811,26 +10773,26 @@
         <v>578</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="J166" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_Video</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_Next</v>
       </c>
       <c r="K166" s="2"/>
       <c r="L166" s="9" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="M166" s="9" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
       <c r="N166" s="5" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A167" s="2" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>112</v>
@@ -10844,27 +10806,27 @@
       <c r="F167" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G167" s="3" t="s">
-        <v>626</v>
+      <c r="G167" s="1" t="s">
+        <v>633</v>
       </c>
       <c r="J167" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_Retry</v>
+        <f t="shared" si="8"/>
+        <v>ZkooTutorialModel_PleaseTapCirclesInOrder</v>
       </c>
       <c r="K167" s="2"/>
       <c r="L167" s="9" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="M167" s="9" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="N167" s="5" t="s">
-        <v>620</v>
+        <v>636</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A168" s="2" t="s">
-        <v>666</v>
+        <v>712</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>112</v>
@@ -10878,27 +10840,27 @@
       <c r="F168" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G168" s="3" t="s">
-        <v>629</v>
+      <c r="G168" s="1" t="s">
+        <v>638</v>
       </c>
       <c r="J168" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_Next</v>
+        <f t="shared" ref="J168:J176" si="9">$F168&amp;IF(ISBLANK($G168),"","_"&amp;$G168)&amp;IF(ISBLANK($H168),"",$H168)&amp;IF(ISBLANK($I168),"","_"&amp;$I168)</f>
+        <v>ZkooTutorialModel_SkipVideo</v>
       </c>
       <c r="K168" s="2"/>
       <c r="L168" s="9" t="s">
-        <v>629</v>
+        <v>639</v>
       </c>
       <c r="M168" s="9" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="N168" s="5" t="s">
-        <v>631</v>
+        <v>641</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A169" s="2" t="s">
-        <v>670</v>
+        <v>716</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>112</v>
@@ -10913,26 +10875,26 @@
         <v>578</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>633</v>
+        <v>643</v>
       </c>
       <c r="J169" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ZkooTutorialModel_PleaseTapCirclesInOrder</v>
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_Complete</v>
       </c>
       <c r="K169" s="2"/>
       <c r="L169" s="9" t="s">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="M169" s="9" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="N169" s="5" t="s">
-        <v>636</v>
+        <v>646</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A170" s="2" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>112</v>
@@ -10947,26 +10909,26 @@
         <v>578</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="J170" s="1" t="str">
-        <f t="shared" ref="J170:J178" si="8">$F170&amp;IF(ISBLANK($G170),"","_"&amp;$G170)&amp;IF(ISBLANK($H170),"",$H170)&amp;IF(ISBLANK($I170),"","_"&amp;$I170)</f>
-        <v>ZkooTutorialModel_SkipVideo</v>
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_TryAgain</v>
       </c>
       <c r="K170" s="2"/>
       <c r="L170" s="9" t="s">
-        <v>639</v>
+        <v>649</v>
       </c>
       <c r="M170" s="9" t="s">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="N170" s="5" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A171" s="2" t="s">
-        <v>716</v>
+        <v>743</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>112</v>
@@ -10981,26 +10943,26 @@
         <v>578</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="J171" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_Complete</v>
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_WellDone</v>
       </c>
       <c r="K171" s="2"/>
       <c r="L171" s="9" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M171" s="9" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="N171" s="5" t="s">
-        <v>646</v>
+        <v>656</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A172" s="2" t="s">
-        <v>717</v>
+        <v>744</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>112</v>
@@ -11015,26 +10977,26 @@
         <v>578</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>648</v>
+        <v>658</v>
       </c>
       <c r="J172" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_TryAgain</v>
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_TutorialCompletes</v>
       </c>
       <c r="K172" s="2"/>
       <c r="L172" s="9" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="M172" s="9" t="s">
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="N172" s="5" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.4">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A173" s="2" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>112</v>
@@ -11049,26 +11011,25 @@
         <v>578</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="J173" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_WellDone</v>
-      </c>
-      <c r="K173" s="2"/>
+        <v>662</v>
+      </c>
+      <c r="J173" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_YouCanStartTutorialFromSettingsBasic</v>
+      </c>
       <c r="L173" s="9" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="M173" s="9" t="s">
-        <v>655</v>
+        <v>664</v>
       </c>
       <c r="N173" s="5" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.4">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A174" s="2" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>112</v>
@@ -11083,26 +11044,25 @@
         <v>578</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="J174" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_TutorialCompletes</v>
-      </c>
-      <c r="K174" s="2"/>
+        <v>667</v>
+      </c>
+      <c r="J174" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_SettingsMenuCanBeOpenedBy</v>
+      </c>
       <c r="L174" s="9" t="s">
-        <v>659</v>
+        <v>668</v>
       </c>
       <c r="M174" s="9" t="s">
-        <v>660</v>
-      </c>
-      <c r="N174" s="5" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
+        <v>669</v>
+      </c>
+      <c r="N174" s="8" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A175" s="2" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>112</v>
@@ -11117,25 +11077,26 @@
         <v>578</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="J175" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_YouCanStartTutorialFromSettingsBasic</v>
-      </c>
+        <v>671</v>
+      </c>
+      <c r="J175" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_StartTutorialAgainWhenZkooApplicationIsLaunched</v>
+      </c>
+      <c r="K175" s="2"/>
       <c r="L175" s="9" t="s">
-        <v>663</v>
+        <v>672</v>
       </c>
       <c r="M175" s="9" t="s">
-        <v>664</v>
+        <v>673</v>
       </c>
       <c r="N175" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" ht="31.5" x14ac:dyDescent="0.4">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="63" x14ac:dyDescent="0.4">
       <c r="A176" s="2" t="s">
-        <v>746</v>
+        <v>798</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>112</v>
@@ -11150,96 +11111,29 @@
         <v>578</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="J176" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_SettingsMenuCanBeOpenedBy</v>
-      </c>
+        <v>747</v>
+      </c>
+      <c r="J176" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>ZkooTutorialModel_TryAgainDetail</v>
+      </c>
+      <c r="K176" s="2"/>
       <c r="L176" s="9" t="s">
-        <v>668</v>
+        <v>748</v>
       </c>
       <c r="M176" s="9" t="s">
-        <v>669</v>
-      </c>
-      <c r="N176" s="8" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A177" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="G177" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="J177" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_StartTutorialAgainWhenZkooApplicationIsLaunched</v>
-      </c>
-      <c r="K177" s="2"/>
-      <c r="L177" s="9" t="s">
-        <v>672</v>
-      </c>
-      <c r="M177" s="9" t="s">
-        <v>673</v>
-      </c>
-      <c r="N177" s="5" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="178" spans="1:14" ht="63" x14ac:dyDescent="0.4">
-      <c r="A178" s="2" t="s">
-        <v>798</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="E178" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="G178" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="J178" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ZkooTutorialModel_TryAgainDetail</v>
-      </c>
-      <c r="K178" s="2"/>
-      <c r="L178" s="9" t="s">
-        <v>748</v>
-      </c>
-      <c r="M178" s="9" t="s">
         <v>749</v>
       </c>
-      <c r="N178" s="12" t="s">
+      <c r="N176" s="12" t="s">
         <v>796</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O139">
-    <sortCondition ref="D2:D139"/>
-    <sortCondition ref="E2:E139"/>
-    <sortCondition ref="F2:F139"/>
-    <sortCondition ref="A2:A139"/>
+  <sortState ref="A2:O137">
+    <sortCondition ref="D2:D137"/>
+    <sortCondition ref="E2:E137"/>
+    <sortCondition ref="F2:F137"/>
+    <sortCondition ref="A2:A137"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11248,14 +11142,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010027AF63008C5B9348B1D80B486CE64D2D" ma:contentTypeVersion="4" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="104485263990d5adc83ab87317f77176">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="86e9103f-040a-4a6c-9c98-6d10a12a6690" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fee4f24d869e615bfcfb8b7a3dd1ece" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11414,7 +11300,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11423,24 +11309,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{489F90DA-672C-4213-BC00-4C8324B9F0A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12BEED70-4FB7-4DEC-BA25-38305F976425}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11459,10 +11336,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A67983-F268-477F-A830-FD85E6BE3CDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{489F90DA-672C-4213-BC00-4C8324B9F0A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix blinking of a selected face area
</commit_message>
<xml_diff>
--- a/Documents/HostApplications_Resources_Strings.xlsx
+++ b/Documents/HostApplications_Resources_Strings.xlsx
@@ -4617,10 +4617,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Max Playable Distance [m]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>最大検出可能距離[m]</t>
     <rPh sb="0" eb="2">
       <t>サイダイ</t>
@@ -4642,6 +4638,10 @@
   </si>
   <si>
     <t>DetectionThreshold</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Max Detectable Distance [m]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5109,9 +5109,9 @@
   <dimension ref="A1:O176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="L85" sqref="L85"/>
+      <selection pane="bottomLeft" activeCell="L117" sqref="L117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7820,7 +7820,7 @@
         <v>113</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="J84" s="1" t="str">
         <f t="shared" si="5"/>
@@ -8996,7 +8996,7 @@
         <v>805</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>821</v>
@@ -9007,13 +9007,13 @@
       </c>
       <c r="K117" s="2"/>
       <c r="L117" s="14" t="s">
+        <v>825</v>
+      </c>
+      <c r="M117" s="14" t="s">
         <v>822</v>
       </c>
-      <c r="M117" s="14" t="s">
-        <v>823</v>
-      </c>
       <c r="N117" s="14" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.4">
@@ -11142,6 +11142,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010027AF63008C5B9348B1D80B486CE64D2D" ma:contentTypeVersion="4" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="104485263990d5adc83ab87317f77176">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="86e9103f-040a-4a6c-9c98-6d10a12a6690" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fee4f24d869e615bfcfb8b7a3dd1ece" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11300,15 +11309,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11318,6 +11318,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A67983-F268-477F-A830-FD85E6BE3CDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12BEED70-4FB7-4DEC-BA25-38305F976425}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11332,14 +11340,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A67983-F268-477F-A830-FD85E6BE3CDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix typos in HostApplications_Resources_Strings.xlsx
</commit_message>
<xml_diff>
--- a/Documents/HostApplications_Resources_Strings.xlsx
+++ b/Documents/HostApplications_Resources_Strings.xlsx
@@ -4526,14 +4526,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MaxPlayableDistanceInMeter</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DetectionThreshold</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Max Detectable Distance [m]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4654,6 +4646,14 @@
   </si>
   <si>
     <t>高灵敏度(易检测)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SensitivityAndSpecificity</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MaxDetectableDistanceInMeter</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5108,10 +5108,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N109" sqref="N109"/>
+      <selection pane="bottomLeft" activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7820,21 +7820,21 @@
         <v>113</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
       <c r="J84" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>CommonStrings_DetectionThreshold</v>
+        <v>CommonStrings_SensitivityAndSpecificity</v>
       </c>
       <c r="K84" s="2"/>
       <c r="L84" s="9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="M84" s="9" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="N84" s="11" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.4">
@@ -7862,13 +7862,13 @@
       </c>
       <c r="K85" s="2"/>
       <c r="L85" s="9" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="M85" s="9" t="s">
         <v>809</v>
       </c>
       <c r="N85" s="11" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.4">
@@ -7896,13 +7896,13 @@
       </c>
       <c r="K86" s="2"/>
       <c r="L86" s="9" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="M86" s="9" t="s">
         <v>808</v>
       </c>
       <c r="N86" s="11" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.4">
@@ -8973,10 +8973,10 @@
         <v>806</v>
       </c>
       <c r="M116" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="N116" s="9" t="s">
         <v>821</v>
-      </c>
-      <c r="N116" s="9" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.4">
@@ -8996,24 +8996,24 @@
         <v>805</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>813</v>
+        <v>826</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>812</v>
       </c>
       <c r="J117" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>EgsDeviceFaceDetectionOnHost_MaxPlayableDistanceInMeter_Description</v>
+        <v>EgsDeviceFaceDetectionOnHost_MaxDetectableDistanceInMeter_Description</v>
       </c>
       <c r="K117" s="2"/>
       <c r="L117" s="9" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="M117" s="9" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="N117" s="9" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.4">
@@ -11142,6 +11142,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010027AF63008C5B9348B1D80B486CE64D2D" ma:contentTypeVersion="4" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="104485263990d5adc83ab87317f77176">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="86e9103f-040a-4a6c-9c98-6d10a12a6690" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fee4f24d869e615bfcfb8b7a3dd1ece" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11300,38 +11317,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12BEED70-4FB7-4DEC-BA25-38305F976425}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A67983-F268-477F-A830-FD85E6BE3CDF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11354,9 +11343,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A67983-F268-477F-A830-FD85E6BE3CDF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12BEED70-4FB7-4DEC-BA25-38305F976425}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>